<commit_message>
Add scheduled sending of emails
</commit_message>
<xml_diff>
--- a/3.0_Software/3.1_Erfassungsseite Dienstleister/Registrierung Diensleister.xlsx
+++ b/3.0_Software/3.1_Erfassungsseite Dienstleister/Registrierung Diensleister.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Registrierung Dienstleister</t>
   </si>
@@ -62,12 +62,6 @@
     <t>Nach Bestätigung</t>
   </si>
   <si>
-    <t>es freut uns sehr, dass Sie sich auf The Eventers.de als Dienstleister registriert haben.</t>
-  </si>
-  <si>
-    <t>Anschließend wählen Sie bitte Ihr Fachgebiet und füllen  das Anmeldeformular vollständig aus.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Um den Vorgang abzuschließen, klicken Sie bitte auf untenstehenden Link. </t>
   </si>
   <si>
@@ -78,13 +72,66 @@
   </si>
   <si>
     <t>Ihr Team von The-Eventers.de</t>
+  </si>
+  <si>
+    <t>Wiederholung E-Mail Adresse</t>
+  </si>
+  <si>
+    <t>Passwort</t>
+  </si>
+  <si>
+    <t>Benutzename (E-Mail Adresse)</t>
+  </si>
+  <si>
+    <t>Passwort bestätigen</t>
+  </si>
+  <si>
+    <t>Anrede</t>
+  </si>
+  <si>
+    <t>Ihr Fachgebiet</t>
+  </si>
+  <si>
+    <t>Anschließend füllen Sie bitte die nötigen Angaben im Anmeldeformular aus.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">vielen Dank, dass Sie sich bei </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Eventers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>als Kooperationspartner registriert haben.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ihr Benutzername ist:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ihr Passwort ist: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +192,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -194,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -229,6 +284,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -544,203 +603,234 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G29"/>
+  <dimension ref="B1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1"/>
     <col min="4" max="4" width="2.85546875" customWidth="1"/>
-    <col min="5" max="5" width="73.7109375" customWidth="1"/>
+    <col min="5" max="5" width="103.42578125" customWidth="1"/>
     <col min="6" max="6" width="2.28515625" customWidth="1"/>
-    <col min="7" max="7" width="88.28515625" customWidth="1"/>
+    <col min="7" max="7" width="91" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F1" s="12"/>
     </row>
-    <row r="2" spans="2:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="12"/>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D3" s="12"/>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="D4" s="12"/>
       <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C5" s="3" t="s">
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D5" s="16"/>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D7" s="16"/>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C7" s="3" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D9" s="16"/>
+      <c r="E9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C9" s="3" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D11" s="16"/>
+      <c r="E11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C11" s="3"/>
-      <c r="D11" s="16"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D12" s="12"/>
       <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D13" s="12"/>
       <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="D14" s="12"/>
       <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D15" s="16"/>
       <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="D16" s="12"/>
       <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D17" s="12"/>
-      <c r="E17" s="7" t="s">
-        <v>15</v>
-      </c>
       <c r="F17" s="13"/>
-      <c r="G17" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="D18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="4:7" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="3:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C19" s="19"/>
       <c r="D19" s="12"/>
-      <c r="E19" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="E19" s="18"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D20" s="12"/>
-      <c r="E20" s="1"/>
       <c r="F20" s="14"/>
-      <c r="G20" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D21" s="12"/>
-      <c r="E21" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="F21" s="15"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="4:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="3:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="12"/>
-      <c r="E22" s="4"/>
       <c r="F22" s="15"/>
-      <c r="G22" s="8" t="s">
+    </row>
+    <row r="23" spans="3:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C23" s="17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="4:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D23" s="12"/>
-      <c r="E23" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="F23" s="15"/>
-      <c r="G23" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="4:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="3:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="12"/>
-      <c r="E24" s="4"/>
       <c r="F24" s="15"/>
-      <c r="G24" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="4:7" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D25" s="12"/>
-      <c r="E25" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="F25" s="15"/>
-      <c r="G25" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="4:7" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D26" s="12"/>
       <c r="E26" s="4"/>
       <c r="F26" s="15"/>
-      <c r="G26" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="4:7" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="4:7" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="G29" s="9"/>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="9"/>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G23" r:id="rId1"/>
+    <hyperlink ref="G12" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>